<commit_message>
upddated exp for ira credit
</commit_message>
<xml_diff>
--- a/InputData/elec/BCpUC/Battery Cost per Unit Cap.xlsx
+++ b/InputData/elec/BCpUC/Battery Cost per Unit Cap.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BCpUC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999D7867-60B9-40C5-9EDF-D7A44AA77B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F6D865-6970-43AC-AAE4-3A52F19D49FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="839" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -505,13 +505,13 @@
     <t>Raw Data (2022 $)</t>
   </si>
   <si>
-    <t>Battery Power Cost per Unit Capacity : NDC</t>
-  </si>
-  <si>
     <t>Time (Year)</t>
   </si>
   <si>
-    <t>Battery Energy Cost per Unit Capacity : NDC</t>
+    <t>Battery Energy Cost per Unit Capacity : MostRecentRun</t>
+  </si>
+  <si>
+    <t>Battery Power Cost per Unit Capacity : MostRecentRun</t>
   </si>
 </sst>
 </file>
@@ -1968,69 +1968,15 @@
     <xf numFmtId="5" fontId="10" fillId="14" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="10" fillId="14" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="63" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -2077,6 +2023,60 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="63" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2224,85 +2224,85 @@
                   <c:v>303546</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>277345</c:v>
+                  <c:v>275720</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>256728</c:v>
+                  <c:v>254008</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>240275</c:v>
+                  <c:v>237399</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>226464</c:v>
+                  <c:v>223663</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>214618</c:v>
+                  <c:v>212018</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>204553</c:v>
+                  <c:v>202332</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>196075</c:v>
+                  <c:v>194107</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>188655</c:v>
+                  <c:v>186872</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>182183</c:v>
+                  <c:v>180500</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>176401</c:v>
+                  <c:v>174745</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>171611</c:v>
+                  <c:v>169959</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>167430</c:v>
+                  <c:v>165780</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>163809</c:v>
+                  <c:v>162166</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>160633</c:v>
+                  <c:v>159002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>157780</c:v>
+                  <c:v>156172</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>155218</c:v>
+                  <c:v>153632</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>152921</c:v>
+                  <c:v>151363</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>150890</c:v>
+                  <c:v>149361</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>149018</c:v>
+                  <c:v>147535</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>147310</c:v>
+                  <c:v>145853</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>145744</c:v>
+                  <c:v>144309</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>144287</c:v>
+                  <c:v>142883</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>142963</c:v>
+                  <c:v>141583</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>141726</c:v>
+                  <c:v>140367</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>140576</c:v>
+                  <c:v>139237</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>139495</c:v>
+                  <c:v>138175</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>138485</c:v>
+                  <c:v>137182</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4911,19 +4911,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:108" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="142" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="165"/>
-      <c r="C1" s="165"/>
-      <c r="D1" s="165"/>
-      <c r="E1" s="165"/>
-      <c r="F1" s="165"/>
-      <c r="G1" s="165"/>
-      <c r="H1" s="165"/>
-      <c r="I1" s="165"/>
-      <c r="J1" s="165"/>
-      <c r="K1" s="165"/>
+      <c r="B1" s="142"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
+      <c r="J1" s="142"/>
+      <c r="K1" s="142"/>
       <c r="M1" s="3" t="s">
         <v>68</v>
       </c>
@@ -5053,12 +5053,12 @@
     </row>
     <row r="4" spans="1:108" s="40" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" s="44"/>
-      <c r="L4" s="166" t="s">
+      <c r="L4" s="143" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:108" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L5" s="167"/>
+      <c r="L5" s="144"/>
     </row>
     <row r="6" spans="1:108" s="40" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H6" s="45"/>
@@ -5090,23 +5090,23 @@
       <c r="B7" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="161" t="s">
+      <c r="C7" s="145" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="161"/>
-      <c r="E7" s="161"/>
-      <c r="F7" s="161"/>
-      <c r="G7" s="161"/>
-      <c r="H7" s="161"/>
-      <c r="I7" s="161"/>
-      <c r="J7" s="161"/>
-      <c r="K7" s="161"/>
-      <c r="L7" s="161"/>
-      <c r="M7" s="161"/>
-      <c r="N7" s="161"/>
-      <c r="O7" s="161"/>
-      <c r="P7" s="161"/>
-      <c r="Q7" s="161"/>
+      <c r="D7" s="145"/>
+      <c r="E7" s="145"/>
+      <c r="F7" s="145"/>
+      <c r="G7" s="145"/>
+      <c r="H7" s="145"/>
+      <c r="I7" s="145"/>
+      <c r="J7" s="145"/>
+      <c r="K7" s="145"/>
+      <c r="L7" s="145"/>
+      <c r="M7" s="145"/>
+      <c r="N7" s="145"/>
+      <c r="O7" s="145"/>
+      <c r="P7" s="145"/>
+      <c r="Q7" s="145"/>
       <c r="R7" s="50"/>
       <c r="S7" s="50"/>
       <c r="T7" s="50"/>
@@ -5124,43 +5124,43 @@
     </row>
     <row r="9" spans="1:108" s="40" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9"/>
-      <c r="B9" s="168" t="s">
+      <c r="B9" s="146" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="169" t="s">
+      <c r="D9" s="147" t="s">
         <v>75</v>
       </c>
-      <c r="E9" s="170"/>
-      <c r="F9" s="171"/>
-      <c r="G9" s="172">
+      <c r="E9" s="148"/>
+      <c r="F9" s="149"/>
+      <c r="G9" s="150">
         <v>2021</v>
       </c>
-      <c r="H9" s="173"/>
-      <c r="I9" s="173"/>
-      <c r="J9" s="173"/>
-      <c r="K9" s="174"/>
-      <c r="L9" s="174"/>
+      <c r="H9" s="151"/>
+      <c r="I9" s="151"/>
+      <c r="J9" s="151"/>
+      <c r="K9" s="152"/>
+      <c r="L9" s="152"/>
     </row>
     <row r="10" spans="1:108" s="40" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="168"/>
+      <c r="B10" s="146"/>
       <c r="D10" s="53" t="s">
         <v>76</v>
       </c>
       <c r="J10" s="52"/>
     </row>
     <row r="11" spans="1:108" s="40" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="168"/>
-      <c r="D11" s="175" t="s">
+      <c r="B11" s="146"/>
+      <c r="D11" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="E11" s="176"/>
-      <c r="F11" s="176"/>
-      <c r="G11" s="176"/>
-      <c r="H11" s="176"/>
-      <c r="I11" s="176"/>
-      <c r="J11" s="176"/>
-      <c r="K11" s="176"/>
-      <c r="L11" s="176"/>
+      <c r="E11" s="154"/>
+      <c r="F11" s="154"/>
+      <c r="G11" s="154"/>
+      <c r="H11" s="154"/>
+      <c r="I11" s="154"/>
+      <c r="J11" s="154"/>
+      <c r="K11" s="154"/>
+      <c r="L11" s="154"/>
       <c r="W11" s="54"/>
       <c r="X11" s="55"/>
       <c r="Y11" s="55"/>
@@ -5168,18 +5168,18 @@
       <c r="AA11" s="55"/>
     </row>
     <row r="12" spans="1:108" s="40" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="168"/>
-      <c r="D12" s="177" t="s">
+      <c r="B12" s="146"/>
+      <c r="D12" s="155" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="178"/>
-      <c r="F12" s="178"/>
-      <c r="G12" s="178"/>
-      <c r="H12" s="178"/>
-      <c r="I12" s="178"/>
-      <c r="J12" s="178"/>
-      <c r="K12" s="178"/>
-      <c r="L12" s="179"/>
+      <c r="E12" s="156"/>
+      <c r="F12" s="156"/>
+      <c r="G12" s="156"/>
+      <c r="H12" s="156"/>
+      <c r="I12" s="156"/>
+      <c r="J12" s="156"/>
+      <c r="K12" s="156"/>
+      <c r="L12" s="157"/>
       <c r="M12" s="56"/>
       <c r="W12" s="54"/>
       <c r="X12" s="55"/>
@@ -5188,16 +5188,16 @@
       <c r="AA12" s="55"/>
     </row>
     <row r="13" spans="1:108" s="40" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="168"/>
-      <c r="D13" s="180"/>
-      <c r="E13" s="181"/>
-      <c r="F13" s="181"/>
-      <c r="G13" s="181"/>
-      <c r="H13" s="181"/>
-      <c r="I13" s="181"/>
-      <c r="J13" s="181"/>
-      <c r="K13" s="181"/>
-      <c r="L13" s="182"/>
+      <c r="B13" s="146"/>
+      <c r="D13" s="158"/>
+      <c r="E13" s="159"/>
+      <c r="F13" s="159"/>
+      <c r="G13" s="159"/>
+      <c r="H13" s="159"/>
+      <c r="I13" s="159"/>
+      <c r="J13" s="159"/>
+      <c r="K13" s="159"/>
+      <c r="L13" s="160"/>
       <c r="W13" s="54"/>
       <c r="X13" s="55"/>
       <c r="Y13" s="55"/>
@@ -5205,49 +5205,49 @@
       <c r="AA13" s="55"/>
     </row>
     <row r="14" spans="1:108" ht="37.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="168"/>
+      <c r="B14" s="146"/>
     </row>
     <row r="15" spans="1:108" x14ac:dyDescent="0.25">
-      <c r="B15" s="168"/>
-      <c r="C15" s="183" t="s">
+      <c r="B15" s="146"/>
+      <c r="C15" s="161" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="183"/>
-      <c r="E15" s="183"/>
-      <c r="F15" s="183"/>
-      <c r="G15" s="183"/>
-      <c r="H15" s="183"/>
-      <c r="I15" s="183"/>
-      <c r="J15" s="183"/>
-      <c r="K15" s="183"/>
-      <c r="L15" s="183"/>
-      <c r="M15" s="183"/>
-      <c r="N15" s="183"/>
-      <c r="O15" s="183"/>
-      <c r="P15" s="183"/>
+      <c r="D15" s="161"/>
+      <c r="E15" s="161"/>
+      <c r="F15" s="161"/>
+      <c r="G15" s="161"/>
+      <c r="H15" s="161"/>
+      <c r="I15" s="161"/>
+      <c r="J15" s="161"/>
+      <c r="K15" s="161"/>
+      <c r="L15" s="161"/>
+      <c r="M15" s="161"/>
+      <c r="N15" s="161"/>
+      <c r="O15" s="161"/>
+      <c r="P15" s="161"/>
       <c r="Q15" s="57"/>
     </row>
     <row r="16" spans="1:108" x14ac:dyDescent="0.25">
-      <c r="B16" s="168"/>
-      <c r="C16" s="183"/>
-      <c r="D16" s="183"/>
-      <c r="E16" s="183"/>
-      <c r="F16" s="183"/>
-      <c r="G16" s="183"/>
-      <c r="H16" s="183"/>
-      <c r="I16" s="183"/>
-      <c r="J16" s="183"/>
-      <c r="K16" s="183"/>
-      <c r="L16" s="183"/>
-      <c r="M16" s="183"/>
-      <c r="N16" s="183"/>
-      <c r="O16" s="183"/>
-      <c r="P16" s="183"/>
+      <c r="B16" s="146"/>
+      <c r="C16" s="161"/>
+      <c r="D16" s="161"/>
+      <c r="E16" s="161"/>
+      <c r="F16" s="161"/>
+      <c r="G16" s="161"/>
+      <c r="H16" s="161"/>
+      <c r="I16" s="161"/>
+      <c r="J16" s="161"/>
+      <c r="K16" s="161"/>
+      <c r="L16" s="161"/>
+      <c r="M16" s="161"/>
+      <c r="N16" s="161"/>
+      <c r="O16" s="161"/>
+      <c r="P16" s="161"/>
     </row>
     <row r="17" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="168"/>
+      <c r="B17" s="146"/>
       <c r="C17" s="58"/>
-      <c r="D17" s="158" t="s">
+      <c r="D17" s="168" t="s">
         <v>80</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -5255,9 +5255,9 @@
       </c>
     </row>
     <row r="18" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="168"/>
+      <c r="B18" s="146"/>
       <c r="C18" s="58"/>
-      <c r="D18" s="159"/>
+      <c r="D18" s="169"/>
       <c r="F18" s="1">
         <v>2021</v>
       </c>
@@ -5350,9 +5350,9 @@
       </c>
     </row>
     <row r="19" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="168"/>
+      <c r="B19" s="146"/>
       <c r="C19" s="58"/>
-      <c r="D19" s="159"/>
+      <c r="D19" s="169"/>
       <c r="E19" t="s">
         <v>82</v>
       </c>
@@ -5448,9 +5448,9 @@
       </c>
     </row>
     <row r="20" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="168"/>
+      <c r="B20" s="146"/>
       <c r="C20" s="58"/>
-      <c r="D20" s="160"/>
+      <c r="D20" s="170"/>
       <c r="E20" t="s">
         <v>83</v>
       </c>
@@ -5546,9 +5546,9 @@
       </c>
     </row>
     <row r="21" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="168"/>
+      <c r="B21" s="146"/>
       <c r="C21" s="58"/>
-      <c r="D21" s="160"/>
+      <c r="D21" s="170"/>
       <c r="E21" t="s">
         <v>84</v>
       </c>
@@ -5644,9 +5644,9 @@
       </c>
     </row>
     <row r="22" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="168"/>
+      <c r="B22" s="146"/>
       <c r="C22" s="58"/>
-      <c r="D22" s="160"/>
+      <c r="D22" s="170"/>
       <c r="F22" s="60"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -5679,18 +5679,18 @@
       <c r="AI22" s="5"/>
     </row>
     <row r="23" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="168"/>
+      <c r="B23" s="146"/>
       <c r="C23" s="58"/>
-      <c r="D23" s="160"/>
+      <c r="D23" s="170"/>
       <c r="E23" s="1" t="s">
         <v>85</v>
       </c>
       <c r="F23" s="60"/>
     </row>
     <row r="24" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="168"/>
+      <c r="B24" s="146"/>
       <c r="C24" s="58"/>
-      <c r="D24" s="160"/>
+      <c r="D24" s="170"/>
       <c r="F24" s="1">
         <v>2021</v>
       </c>
@@ -5783,9 +5783,9 @@
       </c>
     </row>
     <row r="25" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="168"/>
+      <c r="B25" s="146"/>
       <c r="C25" s="58"/>
-      <c r="D25" s="160"/>
+      <c r="D25" s="170"/>
       <c r="E25" t="s">
         <v>82</v>
       </c>
@@ -5881,9 +5881,9 @@
       </c>
     </row>
     <row r="26" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="168"/>
+      <c r="B26" s="146"/>
       <c r="C26" s="58"/>
-      <c r="D26" s="160"/>
+      <c r="D26" s="170"/>
       <c r="E26" t="s">
         <v>83</v>
       </c>
@@ -5979,9 +5979,9 @@
       </c>
     </row>
     <row r="27" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="168"/>
+      <c r="B27" s="146"/>
       <c r="C27" s="58"/>
-      <c r="D27" s="160"/>
+      <c r="D27" s="170"/>
       <c r="E27" t="s">
         <v>84</v>
       </c>
@@ -6077,7 +6077,7 @@
       </c>
     </row>
     <row r="28" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="168"/>
+      <c r="B28" s="146"/>
       <c r="C28" s="58"/>
       <c r="D28" s="58"/>
       <c r="G28" s="5"/>
@@ -6115,7 +6115,7 @@
       <c r="AM28" s="5"/>
     </row>
     <row r="29" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="168"/>
+      <c r="B29" s="146"/>
       <c r="C29" s="58"/>
       <c r="D29" s="58"/>
       <c r="E29" s="1" t="s">
@@ -6157,7 +6157,7 @@
       <c r="AM29" s="5"/>
     </row>
     <row r="30" spans="2:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="168"/>
+      <c r="B30" s="146"/>
       <c r="C30" s="58"/>
       <c r="D30" s="58"/>
       <c r="E30" s="1"/>
@@ -6197,9 +6197,9 @@
       <c r="AM30" s="5"/>
     </row>
     <row r="31" spans="2:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="168"/>
+      <c r="B31" s="146"/>
       <c r="C31" s="58"/>
-      <c r="D31" s="159" t="s">
+      <c r="D31" s="169" t="s">
         <v>87</v>
       </c>
       <c r="E31" s="61" t="s">
@@ -6249,9 +6249,9 @@
       <c r="AM31" s="5"/>
     </row>
     <row r="32" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="168"/>
+      <c r="B32" s="146"/>
       <c r="C32" s="58"/>
-      <c r="D32" s="159"/>
+      <c r="D32" s="169"/>
       <c r="E32" s="66" t="s">
         <v>93</v>
       </c>
@@ -6299,9 +6299,9 @@
       <c r="AM32" s="5"/>
     </row>
     <row r="33" spans="2:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="168"/>
+      <c r="B33" s="146"/>
       <c r="C33" s="58"/>
-      <c r="D33" s="159"/>
+      <c r="D33" s="169"/>
       <c r="E33" s="69" t="s">
         <v>98</v>
       </c>
@@ -6349,9 +6349,9 @@
       <c r="AM33" s="5"/>
     </row>
     <row r="34" spans="2:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="168"/>
+      <c r="B34" s="146"/>
       <c r="C34" s="58"/>
-      <c r="D34" s="159"/>
+      <c r="D34" s="169"/>
       <c r="E34" s="72" t="s">
         <v>100</v>
       </c>
@@ -6399,9 +6399,9 @@
       <c r="AM34" s="5"/>
     </row>
     <row r="35" spans="2:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="168"/>
+      <c r="B35" s="146"/>
       <c r="C35" s="58"/>
-      <c r="D35" s="159"/>
+      <c r="D35" s="169"/>
       <c r="E35" s="69" t="s">
         <v>102</v>
       </c>
@@ -6449,9 +6449,9 @@
       <c r="AM35" s="5"/>
     </row>
     <row r="36" spans="2:74" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="168"/>
+      <c r="B36" s="146"/>
       <c r="C36" s="58"/>
-      <c r="D36" s="159"/>
+      <c r="D36" s="169"/>
       <c r="E36" s="75" t="s">
         <v>104</v>
       </c>
@@ -6538,23 +6538,23 @@
       <c r="AM37" s="5"/>
     </row>
     <row r="38" spans="2:74" s="40" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C38" s="161" t="s">
+      <c r="C38" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="D38" s="161"/>
-      <c r="E38" s="161"/>
-      <c r="F38" s="161"/>
-      <c r="G38" s="161"/>
-      <c r="H38" s="161"/>
-      <c r="I38" s="161"/>
-      <c r="J38" s="161"/>
-      <c r="K38" s="161"/>
-      <c r="L38" s="161"/>
-      <c r="M38" s="161"/>
-      <c r="N38" s="161"/>
-      <c r="O38" s="161"/>
-      <c r="P38" s="161"/>
-      <c r="Q38" s="161"/>
+      <c r="D38" s="145"/>
+      <c r="E38" s="145"/>
+      <c r="F38" s="145"/>
+      <c r="G38" s="145"/>
+      <c r="H38" s="145"/>
+      <c r="I38" s="145"/>
+      <c r="J38" s="145"/>
+      <c r="K38" s="145"/>
+      <c r="L38" s="145"/>
+      <c r="M38" s="145"/>
+      <c r="N38" s="145"/>
+      <c r="O38" s="145"/>
+      <c r="P38" s="145"/>
+      <c r="Q38" s="145"/>
       <c r="R38" s="50"/>
       <c r="S38" s="50"/>
       <c r="T38" s="50"/>
@@ -6687,10 +6687,10 @@
       </c>
     </row>
     <row r="43" spans="2:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="163" t="s">
+      <c r="B43" s="177" t="s">
         <v>61</v>
       </c>
-      <c r="D43" s="158" t="s">
+      <c r="D43" s="168" t="s">
         <v>109</v>
       </c>
       <c r="E43" s="79" t="s">
@@ -6792,8 +6792,8 @@
       </c>
     </row>
     <row r="44" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B44" s="163"/>
-      <c r="D44" s="159"/>
+      <c r="B44" s="177"/>
+      <c r="D44" s="169"/>
       <c r="E44" s="82" t="s">
         <v>93</v>
       </c>
@@ -6893,8 +6893,8 @@
       </c>
     </row>
     <row r="45" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B45" s="163"/>
-      <c r="D45" s="159"/>
+      <c r="B45" s="177"/>
+      <c r="D45" s="169"/>
       <c r="E45" s="83" t="s">
         <v>93</v>
       </c>
@@ -6994,8 +6994,8 @@
       </c>
     </row>
     <row r="46" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B46" s="163"/>
-      <c r="D46" s="160"/>
+      <c r="B46" s="177"/>
+      <c r="D46" s="170"/>
       <c r="E46" s="79" t="s">
         <v>98</v>
       </c>
@@ -7128,8 +7128,8 @@
       <c r="BV46" s="5"/>
     </row>
     <row r="47" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B47" s="163"/>
-      <c r="D47" s="160"/>
+      <c r="B47" s="177"/>
+      <c r="D47" s="170"/>
       <c r="E47" s="79" t="s">
         <v>98</v>
       </c>
@@ -7262,8 +7262,8 @@
       <c r="BV47" s="5"/>
     </row>
     <row r="48" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B48" s="163"/>
-      <c r="D48" s="160"/>
+      <c r="B48" s="177"/>
+      <c r="D48" s="170"/>
       <c r="E48" s="79" t="s">
         <v>98</v>
       </c>
@@ -7396,8 +7396,8 @@
       <c r="BV48" s="5"/>
     </row>
     <row r="49" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B49" s="163"/>
-      <c r="D49" s="160"/>
+      <c r="B49" s="177"/>
+      <c r="D49" s="170"/>
       <c r="E49" s="79" t="s">
         <v>100</v>
       </c>
@@ -7530,8 +7530,8 @@
       <c r="BV49" s="5"/>
     </row>
     <row r="50" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B50" s="163"/>
-      <c r="D50" s="160"/>
+      <c r="B50" s="177"/>
+      <c r="D50" s="170"/>
       <c r="E50" s="79" t="s">
         <v>100</v>
       </c>
@@ -7664,8 +7664,8 @@
       <c r="BV50" s="5"/>
     </row>
     <row r="51" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B51" s="163"/>
-      <c r="D51" s="160"/>
+      <c r="B51" s="177"/>
+      <c r="D51" s="170"/>
       <c r="E51" s="79" t="s">
         <v>100</v>
       </c>
@@ -7798,8 +7798,8 @@
       <c r="BV51" s="5"/>
     </row>
     <row r="52" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B52" s="163"/>
-      <c r="D52" s="160"/>
+      <c r="B52" s="177"/>
+      <c r="D52" s="170"/>
       <c r="E52" s="79" t="s">
         <v>102</v>
       </c>
@@ -7932,8 +7932,8 @@
       <c r="BV52" s="5"/>
     </row>
     <row r="53" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B53" s="163"/>
-      <c r="D53" s="160"/>
+      <c r="B53" s="177"/>
+      <c r="D53" s="170"/>
       <c r="E53" s="79" t="s">
         <v>102</v>
       </c>
@@ -8066,8 +8066,8 @@
       <c r="BV53" s="5"/>
     </row>
     <row r="54" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B54" s="163"/>
-      <c r="D54" s="160"/>
+      <c r="B54" s="177"/>
+      <c r="D54" s="170"/>
       <c r="E54" s="79" t="s">
         <v>102</v>
       </c>
@@ -8200,8 +8200,8 @@
       <c r="BV54" s="5"/>
     </row>
     <row r="55" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B55" s="163"/>
-      <c r="D55" s="160"/>
+      <c r="B55" s="177"/>
+      <c r="D55" s="170"/>
       <c r="E55" s="79" t="s">
         <v>104</v>
       </c>
@@ -8334,8 +8334,8 @@
       <c r="BV55" s="5"/>
     </row>
     <row r="56" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B56" s="163"/>
-      <c r="D56" s="160"/>
+      <c r="B56" s="177"/>
+      <c r="D56" s="170"/>
       <c r="E56" s="79" t="s">
         <v>104</v>
       </c>
@@ -8468,8 +8468,8 @@
       <c r="BV56" s="5"/>
     </row>
     <row r="57" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B57" s="163"/>
-      <c r="D57" s="160"/>
+      <c r="B57" s="177"/>
+      <c r="D57" s="170"/>
       <c r="E57" s="79" t="s">
         <v>104</v>
       </c>
@@ -8602,7 +8602,7 @@
       <c r="BV57" s="5"/>
     </row>
     <row r="58" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B58" s="163"/>
+      <c r="B58" s="177"/>
       <c r="D58" s="58"/>
       <c r="E58" s="82"/>
       <c r="F58" s="82"/>
@@ -8671,7 +8671,7 @@
       <c r="BV58" s="5"/>
     </row>
     <row r="59" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B59" s="163"/>
+      <c r="B59" s="177"/>
       <c r="D59" s="58"/>
       <c r="E59" s="82"/>
       <c r="F59" s="82"/>
@@ -8740,7 +8740,7 @@
       <c r="BV59" s="5"/>
     </row>
     <row r="60" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B60" s="163"/>
+      <c r="B60" s="177"/>
       <c r="D60" s="58"/>
       <c r="E60" s="82"/>
       <c r="F60" s="82"/>
@@ -8809,7 +8809,7 @@
       <c r="BV60" s="5"/>
     </row>
     <row r="61" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B61" s="163"/>
+      <c r="B61" s="177"/>
       <c r="D61" s="84"/>
       <c r="E61" s="82"/>
       <c r="F61" s="82"/>
@@ -8905,8 +8905,8 @@
       </c>
     </row>
     <row r="62" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B62" s="163"/>
-      <c r="D62" s="158" t="s">
+      <c r="B62" s="177"/>
+      <c r="D62" s="168" t="s">
         <v>110</v>
       </c>
       <c r="E62" s="79" t="s">
@@ -9008,8 +9008,8 @@
       </c>
     </row>
     <row r="63" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B63" s="163"/>
-      <c r="D63" s="159"/>
+      <c r="B63" s="177"/>
+      <c r="D63" s="169"/>
       <c r="E63" s="82" t="s">
         <v>93</v>
       </c>
@@ -9109,8 +9109,8 @@
       </c>
     </row>
     <row r="64" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B64" s="163"/>
-      <c r="D64" s="159"/>
+      <c r="B64" s="177"/>
+      <c r="D64" s="169"/>
       <c r="E64" s="83" t="s">
         <v>93</v>
       </c>
@@ -9210,8 +9210,8 @@
       </c>
     </row>
     <row r="65" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B65" s="163"/>
-      <c r="D65" s="160"/>
+      <c r="B65" s="177"/>
+      <c r="D65" s="170"/>
       <c r="E65" s="79" t="s">
         <v>98</v>
       </c>
@@ -9311,8 +9311,8 @@
       </c>
     </row>
     <row r="66" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B66" s="163"/>
-      <c r="D66" s="160"/>
+      <c r="B66" s="177"/>
+      <c r="D66" s="170"/>
       <c r="E66" s="79" t="s">
         <v>98</v>
       </c>
@@ -9412,8 +9412,8 @@
       </c>
     </row>
     <row r="67" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B67" s="163"/>
-      <c r="D67" s="160"/>
+      <c r="B67" s="177"/>
+      <c r="D67" s="170"/>
       <c r="E67" s="79" t="s">
         <v>98</v>
       </c>
@@ -9513,8 +9513,8 @@
       </c>
     </row>
     <row r="68" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B68" s="163"/>
-      <c r="D68" s="160"/>
+      <c r="B68" s="177"/>
+      <c r="D68" s="170"/>
       <c r="E68" s="79" t="s">
         <v>100</v>
       </c>
@@ -9614,8 +9614,8 @@
       </c>
     </row>
     <row r="69" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B69" s="163"/>
-      <c r="D69" s="160"/>
+      <c r="B69" s="177"/>
+      <c r="D69" s="170"/>
       <c r="E69" s="79" t="s">
         <v>100</v>
       </c>
@@ -9715,8 +9715,8 @@
       </c>
     </row>
     <row r="70" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B70" s="163"/>
-      <c r="D70" s="160"/>
+      <c r="B70" s="177"/>
+      <c r="D70" s="170"/>
       <c r="E70" s="79" t="s">
         <v>100</v>
       </c>
@@ -9816,8 +9816,8 @@
       </c>
     </row>
     <row r="71" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B71" s="163"/>
-      <c r="D71" s="160"/>
+      <c r="B71" s="177"/>
+      <c r="D71" s="170"/>
       <c r="E71" s="79" t="s">
         <v>102</v>
       </c>
@@ -9950,8 +9950,8 @@
       <c r="BV71" s="5"/>
     </row>
     <row r="72" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B72" s="163"/>
-      <c r="D72" s="160"/>
+      <c r="B72" s="177"/>
+      <c r="D72" s="170"/>
       <c r="E72" s="79" t="s">
         <v>102</v>
       </c>
@@ -10084,8 +10084,8 @@
       <c r="BV72" s="5"/>
     </row>
     <row r="73" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B73" s="163"/>
-      <c r="D73" s="160"/>
+      <c r="B73" s="177"/>
+      <c r="D73" s="170"/>
       <c r="E73" s="79" t="s">
         <v>102</v>
       </c>
@@ -10218,8 +10218,8 @@
       <c r="BV73" s="5"/>
     </row>
     <row r="74" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B74" s="163"/>
-      <c r="D74" s="160"/>
+      <c r="B74" s="177"/>
+      <c r="D74" s="170"/>
       <c r="E74" s="79" t="s">
         <v>104</v>
       </c>
@@ -10352,8 +10352,8 @@
       <c r="BV74" s="5"/>
     </row>
     <row r="75" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B75" s="163"/>
-      <c r="D75" s="160"/>
+      <c r="B75" s="177"/>
+      <c r="D75" s="170"/>
       <c r="E75" s="79" t="s">
         <v>104</v>
       </c>
@@ -10486,8 +10486,8 @@
       <c r="BV75" s="5"/>
     </row>
     <row r="76" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B76" s="163"/>
-      <c r="D76" s="160"/>
+      <c r="B76" s="177"/>
+      <c r="D76" s="170"/>
       <c r="E76" s="79" t="s">
         <v>104</v>
       </c>
@@ -10620,13 +10620,13 @@
       <c r="BV76" s="5"/>
     </row>
     <row r="77" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B77" s="163"/>
+      <c r="B77" s="177"/>
       <c r="D77" s="84"/>
       <c r="E77" s="82"/>
       <c r="F77" s="82"/>
     </row>
     <row r="78" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B78" s="163"/>
+      <c r="B78" s="177"/>
       <c r="D78" s="40"/>
       <c r="E78" s="85"/>
       <c r="F78" s="85"/>
@@ -10722,8 +10722,8 @@
       </c>
     </row>
     <row r="79" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B79" s="163"/>
-      <c r="D79" s="158" t="s">
+      <c r="B79" s="177"/>
+      <c r="D79" s="168" t="s">
         <v>111</v>
       </c>
       <c r="E79" s="79" t="s">
@@ -10825,8 +10825,8 @@
       <c r="AO79" s="1"/>
     </row>
     <row r="80" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B80" s="163"/>
-      <c r="D80" s="159"/>
+      <c r="B80" s="177"/>
+      <c r="D80" s="169"/>
       <c r="E80" s="82" t="s">
         <v>93</v>
       </c>
@@ -10926,8 +10926,8 @@
       <c r="AO80" s="1"/>
     </row>
     <row r="81" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B81" s="163"/>
-      <c r="D81" s="159"/>
+      <c r="B81" s="177"/>
+      <c r="D81" s="169"/>
       <c r="E81" s="83" t="s">
         <v>93</v>
       </c>
@@ -11027,8 +11027,8 @@
       <c r="AO81" s="1"/>
     </row>
     <row r="82" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B82" s="164"/>
-      <c r="D82" s="160"/>
+      <c r="B82" s="178"/>
+      <c r="D82" s="170"/>
       <c r="E82" s="79" t="s">
         <v>98</v>
       </c>
@@ -11127,8 +11127,8 @@
       </c>
     </row>
     <row r="83" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B83" s="164"/>
-      <c r="D83" s="160"/>
+      <c r="B83" s="178"/>
+      <c r="D83" s="170"/>
       <c r="E83" s="79" t="s">
         <v>98</v>
       </c>
@@ -11227,8 +11227,8 @@
       </c>
     </row>
     <row r="84" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B84" s="164"/>
-      <c r="D84" s="160"/>
+      <c r="B84" s="178"/>
+      <c r="D84" s="170"/>
       <c r="E84" s="79" t="s">
         <v>98</v>
       </c>
@@ -11329,8 +11329,8 @@
       <c r="AL84" s="5"/>
     </row>
     <row r="85" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B85" s="164"/>
-      <c r="D85" s="160"/>
+      <c r="B85" s="178"/>
+      <c r="D85" s="170"/>
       <c r="E85" s="79" t="s">
         <v>100</v>
       </c>
@@ -11431,8 +11431,8 @@
       <c r="AL85" s="5"/>
     </row>
     <row r="86" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B86" s="164"/>
-      <c r="D86" s="160"/>
+      <c r="B86" s="178"/>
+      <c r="D86" s="170"/>
       <c r="E86" s="79" t="s">
         <v>100</v>
       </c>
@@ -11533,8 +11533,8 @@
       <c r="AL86" s="5"/>
     </row>
     <row r="87" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B87" s="164"/>
-      <c r="D87" s="160"/>
+      <c r="B87" s="178"/>
+      <c r="D87" s="170"/>
       <c r="E87" s="79" t="s">
         <v>100</v>
       </c>
@@ -11635,8 +11635,8 @@
       <c r="AL87" s="5"/>
     </row>
     <row r="88" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B88" s="164"/>
-      <c r="D88" s="160"/>
+      <c r="B88" s="178"/>
+      <c r="D88" s="170"/>
       <c r="E88" s="79" t="s">
         <v>102</v>
       </c>
@@ -11737,8 +11737,8 @@
       <c r="AL88" s="5"/>
     </row>
     <row r="89" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B89" s="164"/>
-      <c r="D89" s="160"/>
+      <c r="B89" s="178"/>
+      <c r="D89" s="170"/>
       <c r="E89" s="79" t="s">
         <v>102</v>
       </c>
@@ -11839,8 +11839,8 @@
       <c r="AL89" s="5"/>
     </row>
     <row r="90" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B90" s="164"/>
-      <c r="D90" s="160"/>
+      <c r="B90" s="178"/>
+      <c r="D90" s="170"/>
       <c r="E90" s="79" t="s">
         <v>102</v>
       </c>
@@ -11941,8 +11941,8 @@
       <c r="AL90" s="5"/>
     </row>
     <row r="91" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B91" s="164"/>
-      <c r="D91" s="160"/>
+      <c r="B91" s="178"/>
+      <c r="D91" s="170"/>
       <c r="E91" s="79" t="s">
         <v>104</v>
       </c>
@@ -12043,8 +12043,8 @@
       <c r="AL91" s="5"/>
     </row>
     <row r="92" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B92" s="164"/>
-      <c r="D92" s="160"/>
+      <c r="B92" s="178"/>
+      <c r="D92" s="170"/>
       <c r="E92" s="79" t="s">
         <v>104</v>
       </c>
@@ -12145,8 +12145,8 @@
       <c r="AL92" s="5"/>
     </row>
     <row r="93" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B93" s="164"/>
-      <c r="D93" s="160"/>
+      <c r="B93" s="178"/>
+      <c r="D93" s="170"/>
       <c r="E93" s="79" t="s">
         <v>104</v>
       </c>
@@ -12247,10 +12247,10 @@
       <c r="AL93" s="5"/>
     </row>
     <row r="94" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B94" s="164"/>
+      <c r="B94" s="178"/>
     </row>
     <row r="95" spans="2:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="164"/>
+      <c r="B95" s="178"/>
       <c r="G95" s="1">
         <v>2021</v>
       </c>
@@ -12343,8 +12343,8 @@
       </c>
     </row>
     <row r="96" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B96" s="164"/>
-      <c r="D96" s="158" t="s">
+      <c r="B96" s="178"/>
+      <c r="D96" s="168" t="s">
         <v>112</v>
       </c>
       <c r="E96" s="79" t="s">
@@ -12445,8 +12445,8 @@
       </c>
     </row>
     <row r="97" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B97" s="164"/>
-      <c r="D97" s="159"/>
+      <c r="B97" s="178"/>
+      <c r="D97" s="169"/>
       <c r="E97" s="82" t="s">
         <v>93</v>
       </c>
@@ -12545,8 +12545,8 @@
       </c>
     </row>
     <row r="98" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B98" s="164"/>
-      <c r="D98" s="159"/>
+      <c r="B98" s="178"/>
+      <c r="D98" s="169"/>
       <c r="E98" s="83" t="s">
         <v>93</v>
       </c>
@@ -12645,8 +12645,8 @@
       </c>
     </row>
     <row r="99" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B99" s="164"/>
-      <c r="D99" s="160"/>
+      <c r="B99" s="178"/>
+      <c r="D99" s="170"/>
       <c r="E99" s="79" t="s">
         <v>98</v>
       </c>
@@ -12745,8 +12745,8 @@
       </c>
     </row>
     <row r="100" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B100" s="164"/>
-      <c r="D100" s="160"/>
+      <c r="B100" s="178"/>
+      <c r="D100" s="170"/>
       <c r="E100" s="79" t="s">
         <v>98</v>
       </c>
@@ -12845,8 +12845,8 @@
       </c>
     </row>
     <row r="101" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B101" s="164"/>
-      <c r="D101" s="160"/>
+      <c r="B101" s="178"/>
+      <c r="D101" s="170"/>
       <c r="E101" s="79" t="s">
         <v>98</v>
       </c>
@@ -12945,8 +12945,8 @@
       </c>
     </row>
     <row r="102" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B102" s="164"/>
-      <c r="D102" s="160"/>
+      <c r="B102" s="178"/>
+      <c r="D102" s="170"/>
       <c r="E102" s="79" t="s">
         <v>100</v>
       </c>
@@ -13045,8 +13045,8 @@
       </c>
     </row>
     <row r="103" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B103" s="164"/>
-      <c r="D103" s="160"/>
+      <c r="B103" s="178"/>
+      <c r="D103" s="170"/>
       <c r="E103" s="79" t="s">
         <v>100</v>
       </c>
@@ -13145,8 +13145,8 @@
       </c>
     </row>
     <row r="104" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B104" s="164"/>
-      <c r="D104" s="160"/>
+      <c r="B104" s="178"/>
+      <c r="D104" s="170"/>
       <c r="E104" s="79" t="s">
         <v>100</v>
       </c>
@@ -13245,8 +13245,8 @@
       </c>
     </row>
     <row r="105" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B105" s="164"/>
-      <c r="D105" s="160"/>
+      <c r="B105" s="178"/>
+      <c r="D105" s="170"/>
       <c r="E105" s="79" t="s">
         <v>102</v>
       </c>
@@ -13345,8 +13345,8 @@
       </c>
     </row>
     <row r="106" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B106" s="164"/>
-      <c r="D106" s="160"/>
+      <c r="B106" s="178"/>
+      <c r="D106" s="170"/>
       <c r="E106" s="79" t="s">
         <v>102</v>
       </c>
@@ -13445,8 +13445,8 @@
       </c>
     </row>
     <row r="107" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B107" s="164"/>
-      <c r="D107" s="160"/>
+      <c r="B107" s="178"/>
+      <c r="D107" s="170"/>
       <c r="E107" s="79" t="s">
         <v>102</v>
       </c>
@@ -13545,8 +13545,8 @@
       </c>
     </row>
     <row r="108" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B108" s="164"/>
-      <c r="D108" s="160"/>
+      <c r="B108" s="178"/>
+      <c r="D108" s="170"/>
       <c r="E108" s="79" t="s">
         <v>104</v>
       </c>
@@ -13645,8 +13645,8 @@
       </c>
     </row>
     <row r="109" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B109" s="164"/>
-      <c r="D109" s="160"/>
+      <c r="B109" s="178"/>
+      <c r="D109" s="170"/>
       <c r="E109" s="79" t="s">
         <v>104</v>
       </c>
@@ -13745,8 +13745,8 @@
       </c>
     </row>
     <row r="110" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B110" s="164"/>
-      <c r="D110" s="160"/>
+      <c r="B110" s="178"/>
+      <c r="D110" s="170"/>
       <c r="E110" s="79" t="s">
         <v>104</v>
       </c>
@@ -13845,10 +13845,10 @@
       </c>
     </row>
     <row r="111" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B111" s="164"/>
+      <c r="B111" s="178"/>
     </row>
     <row r="112" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B112" s="164"/>
+      <c r="B112" s="178"/>
       <c r="G112" s="1">
         <v>2021</v>
       </c>
@@ -13941,8 +13941,8 @@
       </c>
     </row>
     <row r="113" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B113" s="164"/>
-      <c r="D113" s="158" t="s">
+      <c r="B113" s="178"/>
+      <c r="D113" s="168" t="s">
         <v>113</v>
       </c>
       <c r="E113" s="79" t="s">
@@ -14044,8 +14044,8 @@
       </c>
     </row>
     <row r="114" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B114" s="164"/>
-      <c r="D114" s="159"/>
+      <c r="B114" s="178"/>
+      <c r="D114" s="169"/>
       <c r="E114" s="82" t="s">
         <v>93</v>
       </c>
@@ -14145,8 +14145,8 @@
       </c>
     </row>
     <row r="115" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B115" s="164"/>
-      <c r="D115" s="159"/>
+      <c r="B115" s="178"/>
+      <c r="D115" s="169"/>
       <c r="E115" s="83" t="s">
         <v>93</v>
       </c>
@@ -14246,8 +14246,8 @@
       </c>
     </row>
     <row r="116" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B116" s="164"/>
-      <c r="D116" s="160"/>
+      <c r="B116" s="178"/>
+      <c r="D116" s="170"/>
       <c r="E116" s="79" t="s">
         <v>98</v>
       </c>
@@ -14347,8 +14347,8 @@
       </c>
     </row>
     <row r="117" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B117" s="164"/>
-      <c r="D117" s="160"/>
+      <c r="B117" s="178"/>
+      <c r="D117" s="170"/>
       <c r="E117" s="79" t="s">
         <v>98</v>
       </c>
@@ -14448,8 +14448,8 @@
       </c>
     </row>
     <row r="118" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B118" s="164"/>
-      <c r="D118" s="160"/>
+      <c r="B118" s="178"/>
+      <c r="D118" s="170"/>
       <c r="E118" s="79" t="s">
         <v>98</v>
       </c>
@@ -14549,8 +14549,8 @@
       </c>
     </row>
     <row r="119" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B119" s="164"/>
-      <c r="D119" s="160"/>
+      <c r="B119" s="178"/>
+      <c r="D119" s="170"/>
       <c r="E119" s="79" t="s">
         <v>100</v>
       </c>
@@ -14650,8 +14650,8 @@
       </c>
     </row>
     <row r="120" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B120" s="164"/>
-      <c r="D120" s="160"/>
+      <c r="B120" s="178"/>
+      <c r="D120" s="170"/>
       <c r="E120" s="79" t="s">
         <v>100</v>
       </c>
@@ -14751,8 +14751,8 @@
       </c>
     </row>
     <row r="121" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B121" s="164"/>
-      <c r="D121" s="160"/>
+      <c r="B121" s="178"/>
+      <c r="D121" s="170"/>
       <c r="E121" s="79" t="s">
         <v>100</v>
       </c>
@@ -14852,8 +14852,8 @@
       </c>
     </row>
     <row r="122" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B122" s="164"/>
-      <c r="D122" s="160"/>
+      <c r="B122" s="178"/>
+      <c r="D122" s="170"/>
       <c r="E122" s="79" t="s">
         <v>102</v>
       </c>
@@ -14953,8 +14953,8 @@
       </c>
     </row>
     <row r="123" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B123" s="164"/>
-      <c r="D123" s="160"/>
+      <c r="B123" s="178"/>
+      <c r="D123" s="170"/>
       <c r="E123" s="79" t="s">
         <v>102</v>
       </c>
@@ -15054,8 +15054,8 @@
       </c>
     </row>
     <row r="124" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B124" s="164"/>
-      <c r="D124" s="160"/>
+      <c r="B124" s="178"/>
+      <c r="D124" s="170"/>
       <c r="E124" s="79" t="s">
         <v>102</v>
       </c>
@@ -15155,8 +15155,8 @@
       </c>
     </row>
     <row r="125" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B125" s="164"/>
-      <c r="D125" s="160"/>
+      <c r="B125" s="178"/>
+      <c r="D125" s="170"/>
       <c r="E125" s="79" t="s">
         <v>104</v>
       </c>
@@ -15256,8 +15256,8 @@
       </c>
     </row>
     <row r="126" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B126" s="164"/>
-      <c r="D126" s="160"/>
+      <c r="B126" s="178"/>
+      <c r="D126" s="170"/>
       <c r="E126" s="79" t="s">
         <v>104</v>
       </c>
@@ -15357,8 +15357,8 @@
       </c>
     </row>
     <row r="127" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B127" s="164"/>
-      <c r="D127" s="160"/>
+      <c r="B127" s="178"/>
+      <c r="D127" s="170"/>
       <c r="E127" s="79" t="s">
         <v>104</v>
       </c>
@@ -15461,23 +15461,23 @@
       <c r="B128" s="87"/>
     </row>
     <row r="129" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B129" s="162" t="s">
+      <c r="B129" s="171" t="s">
         <v>114</v>
       </c>
-      <c r="C129" s="161"/>
-      <c r="D129" s="161"/>
-      <c r="E129" s="161"/>
-      <c r="F129" s="161"/>
-      <c r="G129" s="161"/>
-      <c r="H129" s="161"/>
-      <c r="I129" s="161"/>
-      <c r="J129" s="161"/>
-      <c r="K129" s="161"/>
-      <c r="L129" s="161"/>
-      <c r="M129" s="161"/>
-      <c r="N129" s="161"/>
-      <c r="O129" s="161"/>
-      <c r="P129" s="161"/>
+      <c r="C129" s="145"/>
+      <c r="D129" s="145"/>
+      <c r="E129" s="145"/>
+      <c r="F129" s="145"/>
+      <c r="G129" s="145"/>
+      <c r="H129" s="145"/>
+      <c r="I129" s="145"/>
+      <c r="J129" s="145"/>
+      <c r="K129" s="145"/>
+      <c r="L129" s="145"/>
+      <c r="M129" s="145"/>
+      <c r="N129" s="145"/>
+      <c r="O129" s="145"/>
+      <c r="P129" s="145"/>
       <c r="Q129" s="50"/>
       <c r="R129" s="50"/>
       <c r="S129" s="50"/>
@@ -15512,21 +15512,21 @@
     </row>
     <row r="131" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B131" s="40"/>
-      <c r="C131" s="152" t="s">
+      <c r="C131" s="172" t="s">
         <v>115</v>
       </c>
-      <c r="D131" s="153"/>
-      <c r="E131" s="153"/>
-      <c r="F131" s="153"/>
-      <c r="G131" s="153"/>
-      <c r="H131" s="153"/>
-      <c r="I131" s="155" t="s">
+      <c r="D131" s="173"/>
+      <c r="E131" s="173"/>
+      <c r="F131" s="173"/>
+      <c r="G131" s="173"/>
+      <c r="H131" s="173"/>
+      <c r="I131" s="174" t="s">
         <v>116</v>
       </c>
-      <c r="J131" s="156"/>
-      <c r="K131" s="156"/>
-      <c r="L131" s="156"/>
-      <c r="M131" s="157"/>
+      <c r="J131" s="175"/>
+      <c r="K131" s="175"/>
+      <c r="L131" s="175"/>
+      <c r="M131" s="176"/>
       <c r="N131" s="89" t="s">
         <v>117</v>
       </c>
@@ -15544,14 +15544,14 @@
     </row>
     <row r="132" spans="2:28" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="40"/>
-      <c r="C132" s="142" t="s">
+      <c r="C132" s="162" t="s">
         <v>119</v>
       </c>
-      <c r="D132" s="143"/>
-      <c r="E132" s="143"/>
-      <c r="F132" s="143"/>
-      <c r="G132" s="143"/>
-      <c r="H132" s="144"/>
+      <c r="D132" s="163"/>
+      <c r="E132" s="163"/>
+      <c r="F132" s="163"/>
+      <c r="G132" s="163"/>
+      <c r="H132" s="164"/>
       <c r="I132" t="s">
         <v>95</v>
       </c>
@@ -15562,14 +15562,14 @@
     </row>
     <row r="133" spans="2:28" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B133" s="40"/>
-      <c r="C133" s="142" t="s">
+      <c r="C133" s="162" t="s">
         <v>120</v>
       </c>
-      <c r="D133" s="143"/>
-      <c r="E133" s="143"/>
-      <c r="F133" s="143"/>
-      <c r="G133" s="143"/>
-      <c r="H133" s="144"/>
+      <c r="D133" s="163"/>
+      <c r="E133" s="163"/>
+      <c r="F133" s="163"/>
+      <c r="G133" s="163"/>
+      <c r="H133" s="164"/>
       <c r="I133" s="100" t="s">
         <v>95</v>
       </c>
@@ -15592,21 +15592,21 @@
     </row>
     <row r="134" spans="2:28" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B134" s="40"/>
-      <c r="C134" s="142" t="s">
+      <c r="C134" s="162" t="s">
         <v>109</v>
       </c>
-      <c r="D134" s="143"/>
-      <c r="E134" s="143"/>
-      <c r="F134" s="143"/>
-      <c r="G134" s="143"/>
-      <c r="H134" s="144"/>
-      <c r="I134" s="148" t="s">
+      <c r="D134" s="163"/>
+      <c r="E134" s="163"/>
+      <c r="F134" s="163"/>
+      <c r="G134" s="163"/>
+      <c r="H134" s="164"/>
+      <c r="I134" s="165" t="s">
         <v>122</v>
       </c>
-      <c r="J134" s="149"/>
-      <c r="K134" s="149"/>
-      <c r="L134" s="149"/>
-      <c r="M134" s="150"/>
+      <c r="J134" s="166"/>
+      <c r="K134" s="166"/>
+      <c r="L134" s="166"/>
+      <c r="M134" s="167"/>
       <c r="N134" s="105"/>
       <c r="O134" s="105"/>
       <c r="P134" s="106"/>
@@ -15620,21 +15620,21 @@
     </row>
     <row r="135" spans="2:28" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" s="40"/>
-      <c r="C135" s="142" t="s">
+      <c r="C135" s="162" t="s">
         <v>123</v>
       </c>
-      <c r="D135" s="143"/>
-      <c r="E135" s="143"/>
-      <c r="F135" s="143"/>
-      <c r="G135" s="143"/>
-      <c r="H135" s="144"/>
-      <c r="I135" s="148" t="s">
+      <c r="D135" s="163"/>
+      <c r="E135" s="163"/>
+      <c r="F135" s="163"/>
+      <c r="G135" s="163"/>
+      <c r="H135" s="164"/>
+      <c r="I135" s="165" t="s">
         <v>124</v>
       </c>
-      <c r="J135" s="149"/>
-      <c r="K135" s="149"/>
-      <c r="L135" s="149"/>
-      <c r="M135" s="150"/>
+      <c r="J135" s="166"/>
+      <c r="K135" s="166"/>
+      <c r="L135" s="166"/>
+      <c r="M135" s="167"/>
       <c r="N135" s="105"/>
       <c r="O135" s="105"/>
       <c r="P135" s="106"/>
@@ -15648,14 +15648,14 @@
     </row>
     <row r="136" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B136" s="40"/>
-      <c r="C136" s="142" t="s">
+      <c r="C136" s="162" t="s">
         <v>125</v>
       </c>
-      <c r="D136" s="143"/>
-      <c r="E136" s="143"/>
-      <c r="F136" s="143"/>
-      <c r="G136" s="143"/>
-      <c r="H136" s="144"/>
+      <c r="D136" s="163"/>
+      <c r="E136" s="163"/>
+      <c r="F136" s="163"/>
+      <c r="G136" s="163"/>
+      <c r="H136" s="164"/>
       <c r="I136" s="108" t="s">
         <v>95</v>
       </c>
@@ -15676,14 +15676,14 @@
     </row>
     <row r="137" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B137" s="40"/>
-      <c r="C137" s="145" t="s">
+      <c r="C137" s="179" t="s">
         <v>126</v>
       </c>
-      <c r="D137" s="146"/>
-      <c r="E137" s="146"/>
-      <c r="F137" s="146"/>
-      <c r="G137" s="146"/>
-      <c r="H137" s="147"/>
+      <c r="D137" s="180"/>
+      <c r="E137" s="180"/>
+      <c r="F137" s="180"/>
+      <c r="G137" s="180"/>
+      <c r="H137" s="181"/>
       <c r="I137" s="112" t="s">
         <v>95</v>
       </c>
@@ -15704,12 +15704,12 @@
     </row>
     <row r="138" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B138" s="40"/>
-      <c r="C138" s="151"/>
-      <c r="D138" s="151"/>
-      <c r="E138" s="151"/>
-      <c r="F138" s="151"/>
-      <c r="G138" s="151"/>
-      <c r="H138" s="151"/>
+      <c r="C138" s="182"/>
+      <c r="D138" s="182"/>
+      <c r="E138" s="182"/>
+      <c r="F138" s="182"/>
+      <c r="G138" s="182"/>
+      <c r="H138" s="182"/>
       <c r="I138" s="116"/>
       <c r="J138" s="116"/>
       <c r="K138" s="116"/>
@@ -15728,21 +15728,21 @@
     </row>
     <row r="139" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B139" s="40"/>
-      <c r="C139" s="152" t="s">
+      <c r="C139" s="172" t="s">
         <v>127</v>
       </c>
-      <c r="D139" s="153"/>
-      <c r="E139" s="153"/>
-      <c r="F139" s="153"/>
-      <c r="G139" s="153"/>
-      <c r="H139" s="154"/>
-      <c r="I139" s="155" t="s">
+      <c r="D139" s="173"/>
+      <c r="E139" s="173"/>
+      <c r="F139" s="173"/>
+      <c r="G139" s="173"/>
+      <c r="H139" s="183"/>
+      <c r="I139" s="174" t="s">
         <v>116</v>
       </c>
-      <c r="J139" s="156"/>
-      <c r="K139" s="156"/>
-      <c r="L139" s="156"/>
-      <c r="M139" s="157"/>
+      <c r="J139" s="175"/>
+      <c r="K139" s="175"/>
+      <c r="L139" s="175"/>
+      <c r="M139" s="176"/>
       <c r="N139" s="89" t="s">
         <v>117</v>
       </c>
@@ -15760,14 +15760,14 @@
     </row>
     <row r="140" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B140" s="40"/>
-      <c r="C140" s="142" t="s">
+      <c r="C140" s="162" t="s">
         <v>120</v>
       </c>
-      <c r="D140" s="143"/>
-      <c r="E140" s="143"/>
-      <c r="F140" s="143"/>
-      <c r="G140" s="143"/>
-      <c r="H140" s="144"/>
+      <c r="D140" s="163"/>
+      <c r="E140" s="163"/>
+      <c r="F140" s="163"/>
+      <c r="G140" s="163"/>
+      <c r="H140" s="164"/>
       <c r="I140" s="100" t="s">
         <v>95</v>
       </c>
@@ -15851,14 +15851,14 @@
     </row>
     <row r="143" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B143" s="40"/>
-      <c r="C143" s="142" t="s">
+      <c r="C143" s="162" t="s">
         <v>123</v>
       </c>
-      <c r="D143" s="143"/>
-      <c r="E143" s="143"/>
-      <c r="F143" s="143"/>
-      <c r="G143" s="143"/>
-      <c r="H143" s="144"/>
+      <c r="D143" s="163"/>
+      <c r="E143" s="163"/>
+      <c r="F143" s="163"/>
+      <c r="G143" s="163"/>
+      <c r="H143" s="164"/>
       <c r="I143" s="122" t="s">
         <v>128</v>
       </c>
@@ -15879,14 +15879,14 @@
     </row>
     <row r="144" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B144" s="40"/>
-      <c r="C144" s="142" t="s">
+      <c r="C144" s="162" t="s">
         <v>125</v>
       </c>
-      <c r="D144" s="143"/>
-      <c r="E144" s="143"/>
-      <c r="F144" s="143"/>
-      <c r="G144" s="143"/>
-      <c r="H144" s="144"/>
+      <c r="D144" s="163"/>
+      <c r="E144" s="163"/>
+      <c r="F144" s="163"/>
+      <c r="G144" s="163"/>
+      <c r="H144" s="164"/>
       <c r="I144" s="122" t="s">
         <v>128</v>
       </c>
@@ -15907,14 +15907,14 @@
     </row>
     <row r="145" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B145" s="40"/>
-      <c r="C145" s="145" t="s">
+      <c r="C145" s="179" t="s">
         <v>131</v>
       </c>
-      <c r="D145" s="146"/>
-      <c r="E145" s="146"/>
-      <c r="F145" s="146"/>
-      <c r="G145" s="146"/>
-      <c r="H145" s="147"/>
+      <c r="D145" s="180"/>
+      <c r="E145" s="180"/>
+      <c r="F145" s="180"/>
+      <c r="G145" s="180"/>
+      <c r="H145" s="181"/>
       <c r="I145" s="112" t="s">
         <v>95</v>
       </c>
@@ -16166,16 +16166,17 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="C7:Q7"/>
-    <mergeCell ref="B9:B36"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:L9"/>
-    <mergeCell ref="D11:L11"/>
-    <mergeCell ref="D12:L12"/>
-    <mergeCell ref="D13:L13"/>
-    <mergeCell ref="C15:P16"/>
+    <mergeCell ref="C140:H140"/>
+    <mergeCell ref="C143:H143"/>
+    <mergeCell ref="C144:H144"/>
+    <mergeCell ref="C145:H145"/>
+    <mergeCell ref="C135:H135"/>
+    <mergeCell ref="I135:M135"/>
+    <mergeCell ref="C136:H136"/>
+    <mergeCell ref="C137:H137"/>
+    <mergeCell ref="C138:H138"/>
+    <mergeCell ref="C139:H139"/>
+    <mergeCell ref="I139:M139"/>
     <mergeCell ref="C134:H134"/>
     <mergeCell ref="I134:M134"/>
     <mergeCell ref="D17:D27"/>
@@ -16192,17 +16193,16 @@
     <mergeCell ref="D79:D93"/>
     <mergeCell ref="D96:D110"/>
     <mergeCell ref="D113:D127"/>
-    <mergeCell ref="I135:M135"/>
-    <mergeCell ref="C136:H136"/>
-    <mergeCell ref="C137:H137"/>
-    <mergeCell ref="C138:H138"/>
-    <mergeCell ref="C139:H139"/>
-    <mergeCell ref="I139:M139"/>
-    <mergeCell ref="C140:H140"/>
-    <mergeCell ref="C143:H143"/>
-    <mergeCell ref="C144:H144"/>
-    <mergeCell ref="C145:H145"/>
-    <mergeCell ref="C135:H135"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="C7:Q7"/>
+    <mergeCell ref="B9:B36"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:L9"/>
+    <mergeCell ref="D11:L11"/>
+    <mergeCell ref="D12:L12"/>
+    <mergeCell ref="D13:L13"/>
+    <mergeCell ref="C15:P16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M1" r:id="rId1" display="https://atb.nrel.gov/electricity/2022/utility-scale_battery_storage" xr:uid="{7816EC9A-0454-4087-A6E1-F971C99AA20E}"/>
@@ -17060,17 +17060,17 @@
   <dimension ref="A1:AE12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:AE2"/>
+      <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="47" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B1">
         <v>2021</v>
@@ -17165,7 +17165,7 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2">
         <v>272875</v>
@@ -17177,85 +17177,85 @@
         <v>303546</v>
       </c>
       <c r="E2">
-        <v>277345</v>
+        <v>275720</v>
       </c>
       <c r="F2">
-        <v>256728</v>
+        <v>254008</v>
       </c>
       <c r="G2">
-        <v>240275</v>
+        <v>237399</v>
       </c>
       <c r="H2">
-        <v>226464</v>
+        <v>223663</v>
       </c>
       <c r="I2">
-        <v>214618</v>
+        <v>212018</v>
       </c>
       <c r="J2">
-        <v>204553</v>
+        <v>202332</v>
       </c>
       <c r="K2">
-        <v>196075</v>
+        <v>194107</v>
       </c>
       <c r="L2">
-        <v>188655</v>
+        <v>186872</v>
       </c>
       <c r="M2">
-        <v>182183</v>
+        <v>180500</v>
       </c>
       <c r="N2">
-        <v>176401</v>
+        <v>174745</v>
       </c>
       <c r="O2">
-        <v>171611</v>
+        <v>169959</v>
       </c>
       <c r="P2">
-        <v>167430</v>
+        <v>165780</v>
       </c>
       <c r="Q2">
-        <v>163809</v>
+        <v>162166</v>
       </c>
       <c r="R2">
-        <v>160633</v>
+        <v>159002</v>
       </c>
       <c r="S2">
-        <v>157780</v>
+        <v>156172</v>
       </c>
       <c r="T2">
-        <v>155218</v>
+        <v>153632</v>
       </c>
       <c r="U2">
-        <v>152921</v>
+        <v>151363</v>
       </c>
       <c r="V2">
-        <v>150890</v>
+        <v>149361</v>
       </c>
       <c r="W2">
-        <v>149018</v>
+        <v>147535</v>
       </c>
       <c r="X2">
-        <v>147310</v>
+        <v>145853</v>
       </c>
       <c r="Y2">
-        <v>145744</v>
+        <v>144309</v>
       </c>
       <c r="Z2">
-        <v>144287</v>
+        <v>142883</v>
       </c>
       <c r="AA2">
-        <v>142963</v>
+        <v>141583</v>
       </c>
       <c r="AB2">
-        <v>141726</v>
+        <v>140367</v>
       </c>
       <c r="AC2">
-        <v>140576</v>
+        <v>139237</v>
       </c>
       <c r="AD2">
-        <v>139495</v>
+        <v>138175</v>
       </c>
       <c r="AE2">
-        <v>138485</v>
+        <v>137182</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -17378,7 +17378,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B5">
         <v>2021</v>
@@ -17473,7 +17473,7 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B6">
         <v>253384</v>

</xml_diff>